<commit_message>
Iniziata divisione in componenti degli activity diagram, più sistemazioni footprint dopo revisione prof
</commit_message>
<xml_diff>
--- a/Progetto/ArchLogica.xlsx
+++ b/Progetto/ArchLogica.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Giacomo\IdeaProjects\unimib-software-architecture\Progetto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\g.savazzi\IdeaProjects\unimib-software-architecture-gitlab\Progetto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{418081D9-6DA2-4599-A792-D992BC76C58E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7D34F2-9AEE-42BA-8128-BE36D0754E5D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CE6CBB44-84A0-4BED-899A-38EB3F068B99}"/>
   </bookViews>
@@ -19,17 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -322,9 +311,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -353,6 +339,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -464,16 +453,16 @@
                   <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>50</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>40</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1538,24 +1527,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CBB5A4A-0965-46E8-93F2-7560CFB05C39}">
-  <dimension ref="A1:V19"/>
+  <dimension ref="A1:V23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="V26" sqref="V26"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="4" width="17.7109375" style="1" customWidth="1"/>
-    <col min="19" max="19" width="32.42578125" customWidth="1"/>
-    <col min="20" max="20" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.26953125" customWidth="1"/>
+    <col min="2" max="2" width="15.7265625" customWidth="1"/>
+    <col min="3" max="4" width="17.7265625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="32.453125" customWidth="1"/>
+    <col min="20" max="20" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
@@ -1581,11 +1570,11 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="15" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -1594,324 +1583,327 @@
       <c r="D2" s="4">
         <v>40</v>
       </c>
-      <c r="S2" s="8" t="s">
+      <c r="S2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="8" t="s">
+      <c r="T2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="U2" s="9" t="s">
+      <c r="U2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="V2" s="9">
+      <c r="V2" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="4">
         <v>50</v>
       </c>
-      <c r="S3" s="8" t="s">
+      <c r="S3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="T3" s="8" t="s">
+      <c r="T3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="9" t="s">
+      <c r="U3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="V3" s="9">
+      <c r="V3" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="4">
         <v>30</v>
       </c>
-      <c r="S4" s="8" t="s">
+      <c r="S4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="T4" s="8" t="s">
+      <c r="T4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="U4" s="9" t="s">
+      <c r="U4" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="V4" s="9" t="s">
+      <c r="V4" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="4">
         <v>50</v>
       </c>
-      <c r="S5" s="10" t="s">
+      <c r="S5" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="T5" s="10" t="s">
+      <c r="T5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="U5" s="11" t="s">
+      <c r="U5" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="V5" s="11">
+      <c r="V5" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A6" s="15"/>
+      <c r="B6" s="15"/>
       <c r="C6" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="4">
         <v>40</v>
       </c>
-      <c r="S6" s="10" t="s">
+      <c r="S6" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="T6" s="10" t="s">
+      <c r="T6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="U6" s="11" t="s">
+      <c r="U6" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="V6" s="11">
+      <c r="V6" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A7" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="15" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="4">
-        <v>80</v>
-      </c>
-      <c r="S7" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="S7" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="T7" s="10" t="s">
+      <c r="T7" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="U7" s="11" t="s">
+      <c r="U7" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="V7" s="11" t="s">
+      <c r="V7" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
       <c r="C8" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="4">
-        <v>20</v>
-      </c>
-      <c r="S8" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="S8" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="T8" s="12" t="s">
+      <c r="T8" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="U8" s="13" t="s">
+      <c r="U8" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="V8" s="13">
+      <c r="V8" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
       <c r="C9" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="4">
-        <v>50</v>
-      </c>
-      <c r="S9" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="S9" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="T9" s="12" t="s">
+      <c r="T9" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="U9" s="13" t="s">
+      <c r="U9" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="V9" s="13">
+      <c r="V9" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
       <c r="C10" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="4">
-        <v>40</v>
-      </c>
-      <c r="S10" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="S10" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="T10" s="12" t="s">
+      <c r="T10" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="U10" s="13" t="s">
+      <c r="U10" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="V10" s="13" t="s">
+      <c r="V10" s="12" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="S11" s="14" t="s">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="S11" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="T11" s="14" t="s">
+      <c r="T11" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="U11" s="15" t="s">
+      <c r="U11" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="V11" s="15">
+      <c r="V11" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="S12" s="14" t="s">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="S12" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="T12" s="14" t="s">
+      <c r="T12" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="U12" s="15" t="s">
+      <c r="U12" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="V12" s="15">
+      <c r="V12" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="S13" s="14" t="s">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="S13" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="T13" s="14" t="s">
+      <c r="T13" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="U13" s="15" t="s">
+      <c r="U13" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="V13" s="15">
+      <c r="V13" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="S14" s="14" t="s">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="S14" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="T14" s="14" t="s">
+      <c r="T14" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="U14" s="15" t="s">
+      <c r="U14" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="V14" s="15">
+      <c r="V14" s="14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="S15" s="14" t="s">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="S15" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="T15" s="14" t="s">
+      <c r="T15" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="U15" s="15" t="s">
+      <c r="U15" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="V15" s="15" t="s">
+      <c r="V15" s="14" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="S16" s="6" t="s">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="S16" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="T16" s="6" t="s">
+      <c r="T16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="U16" s="7" t="s">
+      <c r="U16" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="V16" s="7">
+      <c r="V16" s="6">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="19:22" x14ac:dyDescent="0.25">
-      <c r="S17" s="6" t="s">
+    <row r="17" spans="7:22" x14ac:dyDescent="0.35">
+      <c r="S17" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="T17" s="6" t="s">
+      <c r="T17" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="U17" s="7" t="s">
+      <c r="U17" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="V17" s="7">
+      <c r="V17" s="6">
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="19:22" x14ac:dyDescent="0.25">
-      <c r="S18" s="6" t="s">
+    <row r="18" spans="7:22" x14ac:dyDescent="0.35">
+      <c r="S18" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="T18" s="6" t="s">
+      <c r="T18" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="U18" s="7" t="s">
+      <c r="U18" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="V18" s="7">
+      <c r="V18" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="19:22" x14ac:dyDescent="0.25">
-      <c r="S19" s="6" t="s">
+    <row r="19" spans="7:22" x14ac:dyDescent="0.35">
+      <c r="S19" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="T19" s="6" t="s">
+      <c r="T19" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="U19" s="7" t="s">
+      <c r="U19" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="V19" s="7">
+      <c r="V19" s="6">
         <v>5</v>
       </c>
+    </row>
+    <row r="23" spans="7:22" x14ac:dyDescent="0.35">
+      <c r="G23" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Conclusi diagrammi di sequenza.
</commit_message>
<xml_diff>
--- a/Progetto/ArchLogica.xlsx
+++ b/Progetto/ArchLogica.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Giacomo\IdeaProjects\unimib-software-architecture\Progetto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C109072-2FBB-4DDE-9F58-24F85CC19F93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68CBECBC-F513-4315-98E6-29CC0AA05F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CE6CBB44-84A0-4BED-899A-38EB3F068B99}"/>
   </bookViews>
@@ -398,7 +398,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -442,6 +442,9 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -451,10 +454,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1747,7 +1746,7 @@
   <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1768,12 +1767,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1817,10 +1816,10 @@
       <c r="D3" s="8">
         <v>0</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="I3" s="16" t="s">
         <v>9</v>
       </c>
       <c r="J3" s="4" t="s">
@@ -1846,8 +1845,8 @@
       <c r="D4" s="8">
         <v>0</v>
       </c>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
       <c r="J4" s="4" t="s">
         <v>1</v>
       </c>
@@ -1871,8 +1870,8 @@
       <c r="D5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
       <c r="J5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1896,8 +1895,8 @@
       <c r="D6" s="10">
         <v>0</v>
       </c>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
       <c r="J6" s="4" t="s">
         <v>3</v>
       </c>
@@ -1921,8 +1920,8 @@
       <c r="D7" s="10">
         <v>0</v>
       </c>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
       <c r="J7" s="4" t="s">
         <v>4</v>
       </c>
@@ -1946,10 +1945,10 @@
       <c r="D8" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="H8" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="I8" s="16" t="s">
         <v>10</v>
       </c>
       <c r="J8" s="4" t="s">
@@ -1975,8 +1974,8 @@
       <c r="D9" s="12">
         <v>0</v>
       </c>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
       <c r="J9" s="4" t="s">
         <v>6</v>
       </c>
@@ -2000,8 +1999,8 @@
       <c r="D10" s="12">
         <v>0</v>
       </c>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
       <c r="J10" s="4" t="s">
         <v>7</v>
       </c>
@@ -2025,8 +2024,8 @@
       <c r="D11" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
       <c r="J11" s="4" t="s">
         <v>8</v>
       </c>
@@ -2078,9 +2077,6 @@
       <c r="D14" s="14">
         <v>0</v>
       </c>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
     </row>
     <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
@@ -2095,9 +2091,6 @@
       <c r="D15" s="14">
         <v>0</v>
       </c>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
@@ -2170,25 +2163,24 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="18" t="s">
+      <c r="D23" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="G23" s="19"/>
-      <c r="H23" s="20" t="s">
+      <c r="H23" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
     </row>
     <row r="24" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
@@ -2203,7 +2195,6 @@
       <c r="D24" s="8">
         <v>0</v>
       </c>
-      <c r="G24" s="19"/>
       <c r="H24" s="3" t="s">
         <v>13</v>
       </c>
@@ -2233,10 +2224,10 @@
       <c r="D25" s="10">
         <v>0</v>
       </c>
-      <c r="H25" s="15" t="s">
+      <c r="H25" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="I25" s="15" t="s">
+      <c r="I25" s="16" t="s">
         <v>9</v>
       </c>
       <c r="J25" s="4" t="s">
@@ -2262,8 +2253,8 @@
       <c r="D26" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
       <c r="J26" s="4" t="s">
         <v>1</v>
       </c>
@@ -2287,8 +2278,8 @@
       <c r="D27" s="8">
         <v>0</v>
       </c>
-      <c r="H27" s="16"/>
-      <c r="I27" s="16"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
       <c r="J27" s="4" t="s">
         <v>2</v>
       </c>
@@ -2312,8 +2303,8 @@
       <c r="D28" s="10">
         <v>0</v>
       </c>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
       <c r="J28" s="4" t="s">
         <v>3</v>
       </c>
@@ -2337,8 +2328,8 @@
       <c r="D29" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="H29" s="17"/>
-      <c r="I29" s="17"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="18"/>
       <c r="J29" s="4" t="s">
         <v>4</v>
       </c>
@@ -2362,10 +2353,10 @@
       <c r="D30" s="8">
         <v>0</v>
       </c>
-      <c r="H30" s="15" t="s">
+      <c r="H30" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="I30" s="15" t="s">
+      <c r="I30" s="16" t="s">
         <v>10</v>
       </c>
       <c r="J30" s="4" t="s">
@@ -2391,8 +2382,8 @@
       <c r="D31" s="10">
         <v>0</v>
       </c>
-      <c r="H31" s="16"/>
-      <c r="I31" s="16"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
       <c r="J31" s="4" t="s">
         <v>6</v>
       </c>
@@ -2416,8 +2407,8 @@
       <c r="D32" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="H32" s="16"/>
-      <c r="I32" s="16"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
       <c r="J32" s="4" t="s">
         <v>7</v>
       </c>
@@ -2441,8 +2432,8 @@
       <c r="D33" s="8">
         <v>0</v>
       </c>
-      <c r="H33" s="17"/>
-      <c r="I33" s="17"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
       <c r="J33" s="4" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Portata avanti presentazione - savazzi.
</commit_message>
<xml_diff>
--- a/Progetto/ArchLogica.xlsx
+++ b/Progetto/ArchLogica.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Giacomo\IdeaProjects\unimib-software-architecture\Progetto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF47051-851D-4B0D-BA8A-85E11CEC3C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6346C481-76B0-4388-B129-AF14A2D7BB7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CE6CBB44-84A0-4BED-899A-38EB3F068B99}"/>
   </bookViews>
@@ -1746,7 +1746,7 @@
   <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>